<commit_message>
patent and soft fished
</commit_message>
<xml_diff>
--- a/fips/field_map.xlsx
+++ b/fips/field_map.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38265" windowHeight="11325"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38265" windowHeight="11325" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="patent" sheetId="2" r:id="rId1"/>
+    <sheet name="soft" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">patent!$B$1:$I$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">patent!$B$1:$I$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">soft!$B$1:$I$23</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="73">
   <si>
     <t>86_number</t>
   </si>
@@ -150,6 +152,102 @@
   </si>
   <si>
     <t>;</t>
+  </si>
+  <si>
+    <t>patent_inid_72</t>
+  </si>
+  <si>
+    <t>inid_71</t>
+  </si>
+  <si>
+    <t>inid_72</t>
+  </si>
+  <si>
+    <t>inid_73</t>
+  </si>
+  <si>
+    <t>inid_74</t>
+  </si>
+  <si>
+    <t>[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))</t>
+  </si>
+  <si>
+    <t>Номер регистрации (свидетельства)</t>
+  </si>
+  <si>
+    <t>Дата регистрации</t>
+  </si>
+  <si>
+    <t>Номер заявки</t>
+  </si>
+  <si>
+    <t>Дата поступления заявки</t>
+  </si>
+  <si>
+    <t>Дата публикации</t>
+  </si>
+  <si>
+    <t>Контактные реквизиты</t>
+  </si>
+  <si>
+    <t>Автор</t>
+  </si>
+  <si>
+    <t>Правообладатель</t>
+  </si>
+  <si>
+    <t>Название программы ЭВМ/базы данных</t>
+  </si>
+  <si>
+    <t>Тип реализующей ЭВМ</t>
+  </si>
+  <si>
+    <t>Вид и версия системы управления базой данных</t>
+  </si>
+  <si>
+    <t>Вид и версия операционной системы</t>
+  </si>
+  <si>
+    <t>Язык программирования</t>
+  </si>
+  <si>
+    <t>Объем программы для ЭВМ/базы данных</t>
+  </si>
+  <si>
+    <t>Cловесное обозначение вида документа</t>
+  </si>
+  <si>
+    <t>Номер регистрации (свидетельства)_href</t>
+  </si>
+  <si>
+    <t>Дата публикации_href</t>
+  </si>
+  <si>
+    <t>Извещения об изменениях сведений</t>
+  </si>
+  <si>
+    <t>Извещения об изменениях сведений_href</t>
+  </si>
+  <si>
+    <t>soft</t>
+  </si>
+  <si>
+    <t>soft_f_72</t>
+  </si>
+  <si>
+    <t>soft_f_73</t>
+  </si>
+  <si>
+    <t>soft_id</t>
+  </si>
+  <si>
+    <t>[;](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))</t>
+  </si>
+  <si>
+    <t>Программа для ЭВМ/база данных создана по государственному контракту</t>
+  </si>
+  <si>
+    <t>Идентификация органа, регистрирующего программу ЭВМ/базу данных</t>
   </si>
 </sst>
 </file>
@@ -468,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +578,7 @@
     <col min="6" max="6" width="19.140625" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="37.42578125" customWidth="1"/>
     <col min="12" max="12" width="29.42578125" customWidth="1"/>
     <col min="13" max="13" width="35.7109375" customWidth="1"/>
   </cols>
@@ -567,22 +665,22 @@
         <v>31</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E37" si="0">IF(C3="True","inid_"&amp;B3,"f_"&amp;B3)</f>
+        <f t="shared" ref="E3:E39" si="0">IF(C3="True","inid_"&amp;B3,"f_"&amp;B3)</f>
         <v>inid_12</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G37" si="1">IF(F3="patent",1,2)</f>
+        <f t="shared" ref="G3:G39" si="1">IF(F3="patent",1,2)</f>
         <v>1</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" ref="L3:L37" si="2">"{'"&amp;$A$1&amp;"':'"&amp;A3&amp;"',"&amp;"'"&amp;$B$1&amp;"':'"&amp;B3&amp;"',"&amp;"'"&amp;$C$1&amp;"':"&amp;C3&amp;","&amp;"'"&amp;$D$1&amp;"':'"&amp;D3&amp;"',"&amp;"'"&amp;$E$1&amp;"':'"&amp;E3&amp;"',"&amp;"'"&amp;$F$1&amp;"':'"&amp;F3&amp;"',"&amp;"'"&amp;$G$1&amp;"':"&amp;G3&amp;",'"&amp;$H$1&amp;"':'"&amp;H3&amp;"','"&amp;$I$1&amp;"':'"&amp;I3&amp;"','"&amp;$J$1&amp;"':'"&amp;J3&amp;"','"&amp;$K$1&amp;"':'"&amp;K3&amp;"'},"</f>
+        <f t="shared" ref="L3:L39" si="2">"{'"&amp;$A$1&amp;"':'"&amp;A3&amp;"',"&amp;"'"&amp;$B$1&amp;"':'"&amp;B3&amp;"',"&amp;"'"&amp;$C$1&amp;"':"&amp;C3&amp;","&amp;"'"&amp;$D$1&amp;"':'"&amp;D3&amp;"',"&amp;"'"&amp;$E$1&amp;"':'"&amp;E3&amp;"',"&amp;"'"&amp;$F$1&amp;"':'"&amp;F3&amp;"',"&amp;"'"&amp;$G$1&amp;"':"&amp;G3&amp;",'"&amp;$H$1&amp;"':'"&amp;H3&amp;"','"&amp;$I$1&amp;"':'"&amp;I3&amp;"','"&amp;$J$1&amp;"':'"&amp;J3&amp;"','"&amp;$K$1&amp;"':'"&amp;K3&amp;"'},"</f>
         <v>{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
       <c r="M3" t="str">
-        <f t="shared" ref="M3:M37" si="3">M2&amp;L3</f>
+        <f t="shared" ref="M3:M39" si="3">M2&amp;L3</f>
         <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
     </row>
@@ -852,76 +950,76 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B12">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="0"/>
-        <v>inid_54</v>
+        <f t="shared" ref="E12" si="4">IF(C12="True","inid_"&amp;B12,"f_"&amp;B12)</f>
+        <v>inid_48</v>
       </c>
       <c r="F12" t="s">
         <v>4</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G12" si="5">IF(F12="patent",1,2)</f>
         <v>1</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="2"/>
-        <v>{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+        <v>{'doc_field':'48','field_id':'48','inid':True,'field_type':'date','column_name':'inid_48','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+        <f t="shared" ref="M12" si="6">M11&amp;L12</f>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'48','field_id':'48','inid':True,'field_type':'date','column_name':'inid_48','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
+        <v>54</v>
+      </c>
+      <c r="B13">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>inid_54</v>
+      </c>
+      <c r="F13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+      <c r="M13" t="str">
+        <f>M11&amp;L13</f>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>85</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>85</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" t="str">
-        <f t="shared" si="0"/>
-        <v>inid_85</v>
-      </c>
-      <c r="F13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L13" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-      <c r="M13" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1</v>
       </c>
       <c r="C14" t="s">
         <v>27</v>
@@ -931,7 +1029,7 @@
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
-        <v>inid_86_date</v>
+        <v>inid_85</v>
       </c>
       <c r="F14" t="s">
         <v>4</v>
@@ -942,29 +1040,29 @@
       </c>
       <c r="L14" t="str">
         <f t="shared" si="2"/>
-        <v>{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+        <v>{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v>inid_86_number</v>
+        <v>inid_86_date</v>
       </c>
       <c r="F15" t="s">
         <v>4</v>
@@ -975,29 +1073,29 @@
       </c>
       <c r="L15" t="str">
         <f t="shared" si="2"/>
-        <v>{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+        <v>{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
-        <v>inid_87_date</v>
+        <v>inid_86_number</v>
       </c>
       <c r="F16" t="s">
         <v>4</v>
@@ -1008,118 +1106,118 @@
       </c>
       <c r="L16" t="str">
         <f t="shared" si="2"/>
-        <v>{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+        <v>{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>inid_87_date</v>
+      </c>
+      <c r="F17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>2</v>
       </c>
-      <c r="C17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" t="str">
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" t="str">
         <f t="shared" si="0"/>
         <v>inid_87_number</v>
       </c>
-      <c r="F17" t="s">
-        <v>4</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L17" t="str">
+      <c r="F18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L18" t="str">
         <f t="shared" si="2"/>
         <v>{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
-      <c r="M17" t="str">
+      <c r="M18" t="str">
         <f t="shared" si="3"/>
         <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>98</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>98</v>
       </c>
-      <c r="C18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" t="str">
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" t="str">
         <f t="shared" si="0"/>
         <v>f_98</v>
       </c>
-      <c r="F18" t="s">
-        <v>4</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L18" t="str">
+      <c r="F19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L19" t="str">
         <f t="shared" si="2"/>
         <v>{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
-      <c r="M18" t="str">
+      <c r="M19" t="str">
         <f t="shared" si="3"/>
         <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19">
-        <v>121</v>
-      </c>
-      <c r="C19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" t="str">
-        <f t="shared" si="0"/>
-        <v>f_121</v>
-      </c>
-      <c r="F19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L19" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-      <c r="M19" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -1129,7 +1227,7 @@
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
-        <v>f_122</v>
+        <v>f_121</v>
       </c>
       <c r="F20" t="s">
         <v>4</v>
@@ -1140,19 +1238,19 @@
       </c>
       <c r="L20" t="str">
         <f t="shared" si="2"/>
-        <v>{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+        <v>{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C21" t="s">
         <v>28</v>
@@ -1162,7 +1260,7 @@
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
-        <v>f_123</v>
+        <v>f_122</v>
       </c>
       <c r="F21" t="s">
         <v>4</v>
@@ -1173,130 +1271,118 @@
       </c>
       <c r="L21" t="str">
         <f t="shared" si="2"/>
-        <v>{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+        <v>{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>123</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>f_123</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B22">
+      <c r="B23">
         <v>124</v>
       </c>
-      <c r="C22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" t="str">
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" t="str">
         <f t="shared" si="0"/>
         <v>f_124</v>
       </c>
-      <c r="F22" t="s">
-        <v>4</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L22" t="str">
+      <c r="F23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L23" t="str">
         <f t="shared" si="2"/>
         <v>{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
-      <c r="M22" t="str">
+      <c r="M23" t="str">
         <f t="shared" si="3"/>
         <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>126</v>
-      </c>
-      <c r="B23">
-        <v>126</v>
-      </c>
-      <c r="C23" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" t="str">
-        <f t="shared" si="0"/>
-        <v>f_126</v>
-      </c>
-      <c r="F23" t="s">
-        <v>4</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L23" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-      <c r="M23" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>15</v>
+        <v>126</v>
       </c>
       <c r="B24">
-        <v>15</v>
+        <v>126</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D24" t="s">
         <v>31</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
-        <v>inid_15</v>
+        <v>f_126</v>
       </c>
       <c r="F24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H24" t="s">
-        <v>4</v>
-      </c>
-      <c r="I24" t="s">
-        <v>37</v>
-      </c>
-      <c r="J24" t="s">
-        <v>36</v>
-      </c>
-      <c r="K24" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="2"/>
-        <v>{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B25">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
         <v>27</v>
@@ -1306,10 +1392,10 @@
       </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
-        <v>inid_21</v>
+        <v>inid_15</v>
       </c>
       <c r="F25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
@@ -1329,32 +1415,32 @@
       </c>
       <c r="L25" t="str">
         <f t="shared" si="2"/>
-        <v>{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
         <v>27</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
-        <v>inid_22</v>
+        <v>inid_21</v>
       </c>
       <c r="F26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
@@ -1374,19 +1460,19 @@
       </c>
       <c r="L26" t="str">
         <f t="shared" si="2"/>
-        <v>{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
         <v>27</v>
@@ -1396,10 +1482,10 @@
       </c>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
-        <v>inid_23</v>
+        <v>inid_22</v>
       </c>
       <c r="F27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
@@ -1419,32 +1505,32 @@
       </c>
       <c r="L27" t="str">
         <f t="shared" si="2"/>
-        <v>{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B28">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="0"/>
-        <v>inid_30</v>
+        <v>inid_23</v>
       </c>
       <c r="F28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G28">
         <f t="shared" si="1"/>
@@ -1464,19 +1550,19 @@
       </c>
       <c r="L28" t="str">
         <f t="shared" si="2"/>
-        <v>{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s">
         <v>27</v>
@@ -1486,10 +1572,10 @@
       </c>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
-        <v>inid_31</v>
+        <v>inid_30</v>
       </c>
       <c r="F29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
@@ -1509,32 +1595,32 @@
       </c>
       <c r="L29" t="str">
         <f t="shared" si="2"/>
-        <v>{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
         <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
-        <v>inid_32</v>
+        <v>inid_31</v>
       </c>
       <c r="F30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G30">
         <f t="shared" si="1"/>
@@ -1554,32 +1640,32 @@
       </c>
       <c r="L30" t="str">
         <f t="shared" si="2"/>
-        <v>{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B31">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
         <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
-        <v>inid_51</v>
+        <v>inid_32</v>
       </c>
       <c r="F31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
@@ -1599,19 +1685,19 @@
       </c>
       <c r="L31" t="str">
         <f t="shared" si="2"/>
-        <v>{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
       </c>
       <c r="M31" t="str">
         <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B32">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
         <v>27</v>
@@ -1621,10 +1707,10 @@
       </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
-        <v>inid_56</v>
+        <v>inid_51</v>
       </c>
       <c r="F32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
@@ -1644,19 +1730,19 @@
       </c>
       <c r="L32" t="str">
         <f t="shared" si="2"/>
-        <v>{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
       </c>
       <c r="M32" t="str">
         <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B33">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
         <v>27</v>
@@ -1666,10 +1752,10 @@
       </c>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
-        <v>inid_71</v>
+        <v>inid_56</v>
       </c>
       <c r="F33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
@@ -1689,19 +1775,19 @@
       </c>
       <c r="L33" t="str">
         <f t="shared" si="2"/>
-        <v>{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
       </c>
       <c r="M33" t="str">
         <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B34">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
         <v>27</v>
@@ -1709,12 +1795,11 @@
       <c r="D34" t="s">
         <v>31</v>
       </c>
-      <c r="E34" t="str">
-        <f t="shared" si="0"/>
-        <v>inid_73</v>
+      <c r="E34" t="s">
+        <v>42</v>
       </c>
       <c r="F34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
@@ -1730,23 +1815,23 @@
         <v>36</v>
       </c>
       <c r="K34" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="L34" t="str">
         <f t="shared" si="2"/>
-        <v>{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
       </c>
       <c r="M34" t="str">
         <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C35" t="s">
         <v>27</v>
@@ -1754,15 +1839,14 @@
       <c r="D35" t="s">
         <v>31</v>
       </c>
-      <c r="E35" t="str">
-        <f t="shared" si="0"/>
-        <v>inid_74</v>
+      <c r="E35" t="s">
+        <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="G35">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G35" si="7">IF(F35="patent",1,2)</f>
         <v>2</v>
       </c>
       <c r="H35" t="s">
@@ -1775,36 +1859,35 @@
         <v>36</v>
       </c>
       <c r="K35" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="L35" t="str">
         <f t="shared" si="2"/>
-        <v>{'doc_field':'74','field_id':'74','inid':True,'field_type':'string','column_name':'inid_74','table':'patent_inid_74','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>{'doc_field':'72','field_id':'72','inid':True,'field_type':'string','column_name':'inid_72','table':'patent_inid_72','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
       </c>
       <c r="M35" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'74','field_id':'74','inid':True,'field_type':'string','column_name':'inid_74','table':'patent_inid_74','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <f t="shared" ref="M35" si="8">M34&amp;L35</f>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'72','field_id':'72','inid':True,'field_type':'string','column_name':'inid_72','table':'patent_inid_72','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>125</v>
+        <v>73</v>
       </c>
       <c r="B36">
-        <v>125</v>
+        <v>73</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D36" t="s">
         <v>31</v>
       </c>
-      <c r="E36" t="str">
-        <f t="shared" si="0"/>
-        <v>f_125</v>
+      <c r="E36" t="s">
+        <v>44</v>
       </c>
       <c r="F36" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G36">
         <f t="shared" si="1"/>
@@ -1820,52 +1903,141 @@
         <v>36</v>
       </c>
       <c r="K36" t="s">
+        <v>46</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
+      </c>
+      <c r="M36" t="str">
+        <f>M34&amp;L36</f>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>74</v>
+      </c>
+      <c r="B37">
+        <v>74</v>
+      </c>
+      <c r="C37" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H37" t="s">
+        <v>4</v>
+      </c>
+      <c r="I37" t="s">
+        <v>37</v>
+      </c>
+      <c r="J37" t="s">
+        <v>36</v>
+      </c>
+      <c r="K37" t="s">
+        <v>46</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'74','field_id':'74','inid':True,'field_type':'string','column_name':'inid_74','table':'patent_inid_74','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
+      </c>
+      <c r="M37" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'74','field_id':'74','inid':True,'field_type':'string','column_name':'inid_74','table':'patent_inid_74','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>125</v>
+      </c>
+      <c r="B38">
+        <v>125</v>
+      </c>
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" t="s">
+        <v>31</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="0"/>
+        <v>f_125</v>
+      </c>
+      <c r="F38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H38" t="s">
+        <v>4</v>
+      </c>
+      <c r="I38" t="s">
+        <v>37</v>
+      </c>
+      <c r="J38" t="s">
+        <v>36</v>
+      </c>
+      <c r="K38" t="s">
         <v>40</v>
       </c>
-      <c r="L36" t="str">
+      <c r="L38" t="str">
         <f t="shared" si="2"/>
         <v>{'doc_field':'125','field_id':'125','inid':False,'field_type':'string','column_name':'f_125','table':'patent_f_125','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
       </c>
-      <c r="M36" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'74','field_id':'74','inid':True,'field_type':'string','column_name':'inid_74','table':'patent_inid_74','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'125','field_id':'125','inid':False,'field_type':'string','column_name':'f_125','table':'patent_f_125','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="M38" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'74','field_id':'74','inid':True,'field_type':'string','column_name':'inid_74','table':'patent_inid_74','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'125','field_id':'125','inid':False,'field_type':'string','column_name':'f_125','table':'patent_f_125','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>25</v>
       </c>
-      <c r="B37">
+      <c r="B39">
         <v>127</v>
       </c>
-      <c r="C37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D37" t="s">
-        <v>31</v>
-      </c>
-      <c r="E37" t="str">
+      <c r="C39" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39" t="str">
         <f t="shared" si="0"/>
         <v>f_127</v>
       </c>
-      <c r="F37" t="s">
-        <v>4</v>
-      </c>
-      <c r="G37">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L37" t="str">
+      <c r="F39" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L39" t="str">
         <f t="shared" si="2"/>
         <v>{'doc_field':'status','field_id':'127','inid':False,'field_type':'string','column_name':'f_127','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
-      <c r="M37" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'74','field_id':'74','inid':True,'field_type':'string','column_name':'inid_74','table':'patent_inid_74','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'125','field_id':'125','inid':False,'field_type':'string','column_name':'f_125','table':'patent_f_125','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'status','field_id':'127','inid':False,'field_type':'string','column_name':'f_127','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      <c r="M39" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'74','field_id':'74','inid':True,'field_type':'string','column_name':'inid_74','table':'patent_inid_74','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'125','field_id':'125','inid':False,'field_type':'string','column_name':'f_125','table':'patent_f_125','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'status','field_id':'127','inid':False,'field_type':'string','column_name':'f_127','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:I37"/>
+  <autoFilter ref="B1:I39"/>
   <sortState ref="B1:I69">
     <sortCondition ref="F1:F69"/>
     <sortCondition ref="B1:B69"/>
@@ -1873,4 +2045,699 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="71.140625" customWidth="1"/>
+    <col min="2" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="37.42578125" customWidth="1"/>
+    <col min="12" max="12" width="29.42578125" customWidth="1"/>
+    <col min="13" max="13" width="35.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="str">
+        <f>IF(C2="True","inid_"&amp;B2,"f_"&amp;B2)</f>
+        <v>f_11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2">
+        <f>IF(F2="soft",1,2)</f>
+        <v>1</v>
+      </c>
+      <c r="L2" t="str">
+        <f>"{'"&amp;$A$1&amp;"':'"&amp;A2&amp;"',"&amp;"'"&amp;$B$1&amp;"':'"&amp;B2&amp;"',"&amp;"'"&amp;$C$1&amp;"':"&amp;C2&amp;","&amp;"'"&amp;$D$1&amp;"':'"&amp;D2&amp;"',"&amp;"'"&amp;$E$1&amp;"':'"&amp;E2&amp;"',"&amp;"'"&amp;$F$1&amp;"':'"&amp;F2&amp;"',"&amp;"'"&amp;$G$1&amp;"':"&amp;G2&amp;",'"&amp;$H$1&amp;"':'"&amp;H2&amp;"','"&amp;$I$1&amp;"':'"&amp;I2&amp;"','"&amp;$J$1&amp;"':'"&amp;J2&amp;"','"&amp;$K$1&amp;"':'"&amp;K2&amp;"'},"</f>
+        <v>{'doc_field':'Номер регистрации (свидетельства)','field_id':'11','inid':False,'field_type':'string','column_name':'f_11','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E22" si="0">IF(C3="True","inid_"&amp;B3,"f_"&amp;B3)</f>
+        <v>f_12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G22" si="1">IF(F3="soft",1,2)</f>
+        <v>1</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L22" si="2">"{'"&amp;$A$1&amp;"':'"&amp;A3&amp;"',"&amp;"'"&amp;$B$1&amp;"':'"&amp;B3&amp;"',"&amp;"'"&amp;$C$1&amp;"':"&amp;C3&amp;","&amp;"'"&amp;$D$1&amp;"':'"&amp;D3&amp;"',"&amp;"'"&amp;$E$1&amp;"':'"&amp;E3&amp;"',"&amp;"'"&amp;$F$1&amp;"':'"&amp;F3&amp;"',"&amp;"'"&amp;$G$1&amp;"':"&amp;G3&amp;",'"&amp;$H$1&amp;"':'"&amp;H3&amp;"','"&amp;$I$1&amp;"':'"&amp;I3&amp;"','"&amp;$J$1&amp;"':'"&amp;J3&amp;"','"&amp;$K$1&amp;"':'"&amp;K3&amp;"'},"</f>
+        <v>{'doc_field':'Cловесное обозначение вида документа','field_id':'12','inid':False,'field_type':'string','column_name':'f_12','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>f_19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Идентификация органа, регистрирующего программу ЭВМ/базу данных','field_id':'19','inid':False,'field_type':'string','column_name':'f_19','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>f_21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Номер заявки','field_id':'21','inid':False,'field_type':'string','column_name':'f_21','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>f_22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Дата поступления заявки','field_id':'22','inid':False,'field_type':'date','column_name':'f_22','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>f_24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Дата регистрации','field_id':'24','inid':False,'field_type':'date','column_name':'f_24','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>f_45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Дата публикации','field_id':'45','inid':False,'field_type':'date','column_name':'f_45','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>f_54</v>
+      </c>
+      <c r="F9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Название программы ЭВМ/базы данных','field_id':'54','inid':False,'field_type':'string','column_name':'f_54','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10">
+        <v>72</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>f_72</v>
+      </c>
+      <c r="F10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" t="s">
+        <v>70</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Автор','field_id':'72','inid':False,'field_type':'string','column_name':'f_72','table':'soft_f_72','ins_order':2,'ref_table':'soft','ref_field':'id','fk':'soft_id','split_pattern':'[;](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11">
+        <v>73</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>f_73</v>
+      </c>
+      <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" t="s">
+        <v>70</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Правообладатель','field_id':'73','inid':False,'field_type':'string','column_name':'f_73','table':'soft_f_73','ins_order':2,'ref_table':'soft','ref_field':'id','fk':'soft_id','split_pattern':'[;](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12">
+        <v>98</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>f_98</v>
+      </c>
+      <c r="F12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Контактные реквизиты','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13">
+        <v>111</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>f_111</v>
+      </c>
+      <c r="F13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Программа для ЭВМ/база данных создана по государственному контракту','field_id':'111','inid':False,'field_type':'string','column_name':'f_111','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14">
+        <v>112</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>f_112</v>
+      </c>
+      <c r="F14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Вид и версия операционной системы','field_id':'112','inid':False,'field_type':'string','column_name':'f_112','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15">
+        <v>113</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>f_113</v>
+      </c>
+      <c r="F15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Язык программирования','field_id':'113','inid':False,'field_type':'string','column_name':'f_113','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16">
+        <v>114</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>f_114</v>
+      </c>
+      <c r="F16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Вид и версия системы управления базой данных','field_id':'114','inid':False,'field_type':'string','column_name':'f_114','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17">
+        <v>115</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>f_115</v>
+      </c>
+      <c r="F17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Тип реализующей ЭВМ','field_id':'115','inid':False,'field_type':'string','column_name':'f_115','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18">
+        <v>116</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>f_116</v>
+      </c>
+      <c r="F18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Объем программы для ЭВМ/базы данных','field_id':'116','inid':False,'field_type':'string','column_name':'f_116','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19">
+        <v>121</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>f_121</v>
+      </c>
+      <c r="F19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Номер регистрации (свидетельства)_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20">
+        <v>124</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>f_124</v>
+      </c>
+      <c r="F20" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Дата публикации_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21">
+        <v>125</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>f_125</v>
+      </c>
+      <c r="F21" t="s">
+        <v>66</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Извещения об изменениях сведений','field_id':'125','inid':False,'field_type':'string','column_name':'f_125','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22">
+        <v>126</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>f_126</v>
+      </c>
+      <c r="F22" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Извещения об изменениях сведений_href','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:I23"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
return to natural index (document id) solve duplicates in document id
</commit_message>
<xml_diff>
--- a/fips/field_map.xlsx
+++ b/fips/field_map.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="75">
   <si>
     <t>86_number</t>
   </si>
@@ -142,9 +142,6 @@
     <t>patent_id</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>fk</t>
   </si>
   <si>
@@ -248,6 +245,15 @@
   </si>
   <si>
     <t>Идентификация органа, регистрирующего программу ЭВМ/базу данных</t>
+  </si>
+  <si>
+    <t>inid_11_id</t>
+  </si>
+  <si>
+    <t>as_id</t>
+  </si>
+  <si>
+    <t>f_11_id</t>
   </si>
 </sst>
 </file>
@@ -284,8 +290,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -566,25 +573,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26:I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" customWidth="1"/>
     <col min="11" max="11" width="37.42578125" customWidth="1"/>
-    <col min="12" max="12" width="29.42578125" customWidth="1"/>
-    <col min="13" max="13" width="35.7109375" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" customWidth="1"/>
+    <col min="13" max="13" width="29.42578125" customWidth="1"/>
+    <col min="14" max="14" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B1" t="s">
@@ -612,14 +621,17 @@
         <v>35</v>
       </c>
       <c r="J1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s">
         <v>38</v>
       </c>
-      <c r="K1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="L1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>11</v>
       </c>
       <c r="B2">
@@ -642,17 +654,20 @@
         <f>IF(F2="patent",1,2)</f>
         <v>1</v>
       </c>
-      <c r="L2" t="str">
-        <f>"{'"&amp;$A$1&amp;"':'"&amp;A2&amp;"',"&amp;"'"&amp;$B$1&amp;"':'"&amp;B2&amp;"',"&amp;"'"&amp;$C$1&amp;"':"&amp;C2&amp;","&amp;"'"&amp;$D$1&amp;"':'"&amp;D2&amp;"',"&amp;"'"&amp;$E$1&amp;"':'"&amp;E2&amp;"',"&amp;"'"&amp;$F$1&amp;"':'"&amp;F2&amp;"',"&amp;"'"&amp;$G$1&amp;"':"&amp;G2&amp;",'"&amp;$H$1&amp;"':'"&amp;H2&amp;"','"&amp;$I$1&amp;"':'"&amp;I2&amp;"','"&amp;$J$1&amp;"':'"&amp;J2&amp;"','"&amp;$K$1&amp;"':'"&amp;K2&amp;"'},"</f>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      <c r="L2">
+        <v>1</v>
       </c>
       <c r="M2" t="str">
-        <f>M1&amp;L2</f>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3">
+        <f>"{'"&amp;$A$1&amp;"':'"&amp;A2&amp;"',"&amp;"'"&amp;$B$1&amp;"':'"&amp;B2&amp;"',"&amp;"'"&amp;$C$1&amp;"':"&amp;C2&amp;","&amp;"'"&amp;$D$1&amp;"':'"&amp;D2&amp;"',"&amp;"'"&amp;$E$1&amp;"':'"&amp;E2&amp;"',"&amp;"'"&amp;$F$1&amp;"':'"&amp;F2&amp;"',"&amp;"'"&amp;$G$1&amp;"':"&amp;G2&amp;",'"&amp;$H$1&amp;"':'"&amp;H2&amp;"','"&amp;$I$1&amp;"':'"&amp;I2&amp;"','"&amp;$J$1&amp;"':'"&amp;J2&amp;"','"&amp;$K$1&amp;"':'"&amp;K2&amp;"','"&amp;$L$1&amp;"':'"&amp;L2&amp;"'},"</f>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},</v>
+      </c>
+      <c r="N2" t="str">
+        <f>N1&amp;M2</f>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>12</v>
       </c>
       <c r="B3">
@@ -675,17 +690,17 @@
         <f t="shared" ref="G3:G39" si="1">IF(F3="patent",1,2)</f>
         <v>1</v>
       </c>
-      <c r="L3" t="str">
-        <f t="shared" ref="L3:L39" si="2">"{'"&amp;$A$1&amp;"':'"&amp;A3&amp;"',"&amp;"'"&amp;$B$1&amp;"':'"&amp;B3&amp;"',"&amp;"'"&amp;$C$1&amp;"':"&amp;C3&amp;","&amp;"'"&amp;$D$1&amp;"':'"&amp;D3&amp;"',"&amp;"'"&amp;$E$1&amp;"':'"&amp;E3&amp;"',"&amp;"'"&amp;$F$1&amp;"':'"&amp;F3&amp;"',"&amp;"'"&amp;$G$1&amp;"':"&amp;G3&amp;",'"&amp;$H$1&amp;"':'"&amp;H3&amp;"','"&amp;$I$1&amp;"':'"&amp;I3&amp;"','"&amp;$J$1&amp;"':'"&amp;J3&amp;"','"&amp;$K$1&amp;"':'"&amp;K3&amp;"'},"</f>
-        <v>{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M3" t="str">
-        <f t="shared" ref="M3:M39" si="3">M2&amp;L3</f>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4">
+        <f t="shared" ref="M3:M39" si="2">"{'"&amp;$A$1&amp;"':'"&amp;A3&amp;"',"&amp;"'"&amp;$B$1&amp;"':'"&amp;B3&amp;"',"&amp;"'"&amp;$C$1&amp;"':"&amp;C3&amp;","&amp;"'"&amp;$D$1&amp;"':'"&amp;D3&amp;"',"&amp;"'"&amp;$E$1&amp;"':'"&amp;E3&amp;"',"&amp;"'"&amp;$F$1&amp;"':'"&amp;F3&amp;"',"&amp;"'"&amp;$G$1&amp;"':"&amp;G3&amp;",'"&amp;$H$1&amp;"':'"&amp;H3&amp;"','"&amp;$I$1&amp;"':'"&amp;I3&amp;"','"&amp;$J$1&amp;"':'"&amp;J3&amp;"','"&amp;$K$1&amp;"':'"&amp;K3&amp;"','"&amp;$L$1&amp;"':'"&amp;L3&amp;"'},"</f>
+        <v>{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N39" si="3">N2&amp;M3</f>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>13</v>
       </c>
       <c r="B4">
@@ -708,17 +723,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L4" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M4" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>19</v>
       </c>
       <c r="B5">
@@ -741,17 +756,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L5" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M5" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>24</v>
       </c>
       <c r="B6">
@@ -774,17 +789,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L6" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M6" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>33</v>
       </c>
       <c r="B7">
@@ -807,17 +822,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L7" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M7" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>41</v>
       </c>
       <c r="B8">
@@ -840,17 +855,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L8" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M8" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>43</v>
       </c>
       <c r="B9">
@@ -873,17 +888,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L9" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M9" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>45</v>
       </c>
       <c r="B10">
@@ -906,17 +921,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L10" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M10" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>46</v>
       </c>
       <c r="B11">
@@ -939,17 +954,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L11" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M11" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>48</v>
       </c>
       <c r="B12">
@@ -972,17 +987,17 @@
         <f t="shared" ref="G12" si="5">IF(F12="patent",1,2)</f>
         <v>1</v>
       </c>
-      <c r="L12" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'48','field_id':'48','inid':True,'field_type':'date','column_name':'inid_48','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M12" t="str">
-        <f t="shared" ref="M12" si="6">M11&amp;L12</f>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'48','field_id':'48','inid':True,'field_type':'date','column_name':'inid_48','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'48','field_id':'48','inid':True,'field_type':'date','column_name':'inid_48','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" ref="N12" si="6">N11&amp;M12</f>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'48','field_id':'48','inid':True,'field_type':'date','column_name':'inid_48','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>54</v>
       </c>
       <c r="B13">
@@ -1005,17 +1020,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L13" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M13" t="str">
-        <f>M11&amp;L13</f>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N13" t="str">
+        <f>N11&amp;M13</f>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>85</v>
       </c>
       <c r="B14">
@@ -1038,17 +1053,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L14" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M14" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B15" t="s">
@@ -1071,17 +1086,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L15" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M15" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B16" t="s">
@@ -1104,17 +1119,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L16" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M16" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B17" t="s">
@@ -1137,17 +1152,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L17" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M17" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B18" t="s">
@@ -1170,17 +1185,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L18" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M18" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>98</v>
       </c>
       <c r="B19">
@@ -1203,17 +1218,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L19" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M19" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20">
@@ -1236,17 +1251,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L20" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M20" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B21">
@@ -1269,17 +1284,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L21" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M21" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B22">
@@ -1302,17 +1317,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L22" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M22" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B23">
@@ -1335,17 +1350,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L23" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M23" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>126</v>
       </c>
       <c r="B24">
@@ -1368,17 +1383,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L24" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M24" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>15</v>
       </c>
       <c r="B25">
@@ -1405,25 +1420,25 @@
         <v>4</v>
       </c>
       <c r="I25" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="J25" t="s">
         <v>36</v>
       </c>
       <c r="K25" t="s">
-        <v>40</v>
-      </c>
-      <c r="L25" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>39</v>
       </c>
       <c r="M25" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>21</v>
       </c>
       <c r="B26">
@@ -1450,25 +1465,25 @@
         <v>4</v>
       </c>
       <c r="I26" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="J26" t="s">
         <v>36</v>
       </c>
       <c r="K26" t="s">
-        <v>40</v>
-      </c>
-      <c r="L26" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>39</v>
       </c>
       <c r="M26" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>22</v>
       </c>
       <c r="B27">
@@ -1495,25 +1510,25 @@
         <v>4</v>
       </c>
       <c r="I27" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="J27" t="s">
         <v>36</v>
       </c>
       <c r="K27" t="s">
-        <v>40</v>
-      </c>
-      <c r="L27" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>39</v>
       </c>
       <c r="M27" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+      <c r="N27" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>23</v>
       </c>
       <c r="B28">
@@ -1540,25 +1555,25 @@
         <v>4</v>
       </c>
       <c r="I28" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="J28" t="s">
         <v>36</v>
       </c>
       <c r="K28" t="s">
-        <v>40</v>
-      </c>
-      <c r="L28" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>39</v>
       </c>
       <c r="M28" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+      <c r="N28" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>30</v>
       </c>
       <c r="B29">
@@ -1585,25 +1600,25 @@
         <v>4</v>
       </c>
       <c r="I29" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="J29" t="s">
         <v>36</v>
       </c>
       <c r="K29" t="s">
-        <v>40</v>
-      </c>
-      <c r="L29" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>39</v>
       </c>
       <c r="M29" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+      <c r="N29" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>31</v>
       </c>
       <c r="B30">
@@ -1630,25 +1645,25 @@
         <v>4</v>
       </c>
       <c r="I30" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="J30" t="s">
         <v>36</v>
       </c>
       <c r="K30" t="s">
-        <v>40</v>
-      </c>
-      <c r="L30" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>39</v>
       </c>
       <c r="M30" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+      <c r="N30" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>32</v>
       </c>
       <c r="B31">
@@ -1675,25 +1690,25 @@
         <v>4</v>
       </c>
       <c r="I31" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="J31" t="s">
         <v>36</v>
       </c>
       <c r="K31" t="s">
-        <v>40</v>
-      </c>
-      <c r="L31" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>39</v>
       </c>
       <c r="M31" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+      <c r="N31" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>51</v>
       </c>
       <c r="B32">
@@ -1720,25 +1735,25 @@
         <v>4</v>
       </c>
       <c r="I32" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="J32" t="s">
         <v>36</v>
       </c>
       <c r="K32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L32" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>39</v>
       </c>
       <c r="M32" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+      <c r="N32" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>56</v>
       </c>
       <c r="B33">
@@ -1765,25 +1780,25 @@
         <v>4</v>
       </c>
       <c r="I33" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="J33" t="s">
         <v>36</v>
       </c>
       <c r="K33" t="s">
-        <v>40</v>
-      </c>
-      <c r="L33" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>39</v>
       </c>
       <c r="M33" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+      <c r="N33" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>71</v>
       </c>
       <c r="B34">
@@ -1796,7 +1811,7 @@
         <v>31</v>
       </c>
       <c r="E34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F34" t="s">
         <v>14</v>
@@ -1809,25 +1824,25 @@
         <v>4</v>
       </c>
       <c r="I34" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="J34" t="s">
         <v>36</v>
       </c>
       <c r="K34" t="s">
-        <v>46</v>
-      </c>
-      <c r="L34" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
+        <v>45</v>
       </c>
       <c r="M34" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},</v>
+      </c>
+      <c r="N34" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>72</v>
       </c>
       <c r="B35">
@@ -1840,10 +1855,10 @@
         <v>31</v>
       </c>
       <c r="E35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G35">
         <f t="shared" ref="G35" si="7">IF(F35="patent",1,2)</f>
@@ -1853,25 +1868,25 @@
         <v>4</v>
       </c>
       <c r="I35" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="J35" t="s">
         <v>36</v>
       </c>
       <c r="K35" t="s">
-        <v>46</v>
-      </c>
-      <c r="L35" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'72','field_id':'72','inid':True,'field_type':'string','column_name':'inid_72','table':'patent_inid_72','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
+        <v>45</v>
       </c>
       <c r="M35" t="str">
-        <f t="shared" ref="M35" si="8">M34&amp;L35</f>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'72','field_id':'72','inid':True,'field_type':'string','column_name':'inid_72','table':'patent_inid_72','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'72','field_id':'72','inid':True,'field_type':'string','column_name':'inid_72','table':'patent_inid_72','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},</v>
+      </c>
+      <c r="N35" t="str">
+        <f t="shared" ref="N35" si="8">N34&amp;M35</f>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},{'doc_field':'72','field_id':'72','inid':True,'field_type':'string','column_name':'inid_72','table':'patent_inid_72','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>73</v>
       </c>
       <c r="B36">
@@ -1884,7 +1899,7 @@
         <v>31</v>
       </c>
       <c r="E36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F36" t="s">
         <v>15</v>
@@ -1897,25 +1912,25 @@
         <v>4</v>
       </c>
       <c r="I36" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="J36" t="s">
         <v>36</v>
       </c>
       <c r="K36" t="s">
-        <v>46</v>
-      </c>
-      <c r="L36" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
+        <v>45</v>
       </c>
       <c r="M36" t="str">
-        <f>M34&amp;L36</f>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},</v>
+      </c>
+      <c r="N36" t="str">
+        <f>N34&amp;M36</f>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>74</v>
       </c>
       <c r="B37">
@@ -1928,7 +1943,7 @@
         <v>31</v>
       </c>
       <c r="E37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F37" t="s">
         <v>16</v>
@@ -1941,25 +1956,25 @@
         <v>4</v>
       </c>
       <c r="I37" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="J37" t="s">
         <v>36</v>
       </c>
       <c r="K37" t="s">
-        <v>46</v>
-      </c>
-      <c r="L37" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'74','field_id':'74','inid':True,'field_type':'string','column_name':'inid_74','table':'patent_inid_74','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
+        <v>45</v>
       </c>
       <c r="M37" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'74','field_id':'74','inid':True,'field_type':'string','column_name':'inid_74','table':'patent_inid_74','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'74','field_id':'74','inid':True,'field_type':'string','column_name':'inid_74','table':'patent_inid_74','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},</v>
+      </c>
+      <c r="N37" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},{'doc_field':'74','field_id':'74','inid':True,'field_type':'string','column_name':'inid_74','table':'patent_inid_74','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>125</v>
       </c>
       <c r="B38">
@@ -1986,25 +2001,25 @@
         <v>4</v>
       </c>
       <c r="I38" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="J38" t="s">
         <v>36</v>
       </c>
       <c r="K38" t="s">
-        <v>40</v>
-      </c>
-      <c r="L38" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'125','field_id':'125','inid':False,'field_type':'string','column_name':'f_125','table':'patent_f_125','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
+        <v>39</v>
       </c>
       <c r="M38" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'74','field_id':'74','inid':True,'field_type':'string','column_name':'inid_74','table':'patent_inid_74','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'125','field_id':'125','inid':False,'field_type':'string','column_name':'f_125','table':'patent_f_125','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'125','field_id':'125','inid':False,'field_type':'string','column_name':'f_125','table':'patent_f_125','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+      <c r="N38" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},{'doc_field':'74','field_id':'74','inid':True,'field_type':'string','column_name':'inid_74','table':'patent_inid_74','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},{'doc_field':'125','field_id':'125','inid':False,'field_type':'string','column_name':'f_125','table':'patent_f_125','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B39">
@@ -2027,13 +2042,13 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L39" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'status','field_id':'127','inid':False,'field_type':'string','column_name':'f_127','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
       <c r="M39" t="str">
-        <f t="shared" si="3"/>
-        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'74','field_id':'74','inid':True,'field_type':'string','column_name':'inid_74','table':'patent_inid_74','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},{'doc_field':'125','field_id':'125','inid':False,'field_type':'string','column_name':'f_125','table':'patent_f_125','ins_order':2,'ref_table':'patent','ref_field':'id','fk':'patent_id','split_pattern':';'},{'doc_field':'status','field_id':'127','inid':False,'field_type':'string','column_name':'f_127','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'status','field_id':'127','inid':False,'field_type':'string','column_name':'f_127','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+      <c r="N39" t="str">
+        <f t="shared" si="3"/>
+        <v>{'doc_field':'11','field_id':'11','inid':True,'field_type':'string','column_name':'inid_11','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},{'doc_field':'12','field_id':'12','inid':True,'field_type':'string','column_name':'inid_12','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'13','field_id':'13','inid':True,'field_type':'string','column_name':'inid_13','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'19','field_id':'19','inid':True,'field_type':'string','column_name':'inid_19','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'24','field_id':'24','inid':True,'field_type':'date','column_name':'inid_24','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'33','field_id':'33','inid':True,'field_type':'string','column_name':'inid_33','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'41','field_id':'41','inid':True,'field_type':'date','column_name':'inid_41','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43','field_id':'43','inid':True,'field_type':'date','column_name':'inid_43','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45','field_id':'45','inid':True,'field_type':'date','column_name':'inid_45','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'46','field_id':'46','inid':True,'field_type':'date','column_name':'inid_46','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'54','field_id':'54','inid':True,'field_type':'string','column_name':'inid_54','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'85','field_id':'85','inid':True,'field_type':'date','column_name':'inid_85','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_date','field_id':'86_date','inid':True,'field_type':'date','column_name':'inid_86_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'86_number','field_id':'86_number','inid':True,'field_type':'string','column_name':'inid_86_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_date','field_id':'87_date','inid':True,'field_type':'date','column_name':'inid_87_date','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'87_number','field_id':'87_number','inid':True,'field_type':'string','column_name':'inid_87_number','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'98','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'11_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'21_href','field_id':'122','inid':False,'field_type':'string','column_name':'f_122','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'43_href','field_id':'123','inid':False,'field_type':'string','column_name':'f_123','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'45_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'126','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},{'doc_field':'15','field_id':'15','inid':True,'field_type':'string','column_name':'inid_15','table':'patent_inid_15','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'21','field_id':'21','inid':True,'field_type':'string','column_name':'inid_21','table':'patent_inid_21','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'22','field_id':'22','inid':True,'field_type':'date','column_name':'inid_22','table':'patent_inid_22','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'23','field_id':'23','inid':True,'field_type':'date','column_name':'inid_23','table':'patent_inid_23','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'30','field_id':'30','inid':True,'field_type':'string','column_name':'inid_30','table':'patent_inid_30','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'31','field_id':'31','inid':True,'field_type':'string','column_name':'inid_31','table':'patent_inid_31','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'32','field_id':'32','inid':True,'field_type':'date','column_name':'inid_32','table':'patent_inid_32','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'51','field_id':'51','inid':True,'field_type':'string','column_name':'inid_51','table':'patent_inid_51','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'56','field_id':'56','inid':True,'field_type':'string','column_name':'inid_56','table':'patent_inid_56','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'71','field_id':'71','inid':True,'field_type':'string','column_name':'inid_71','table':'patent_inid_71','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},{'doc_field':'73','field_id':'73','inid':True,'field_type':'string','column_name':'inid_73','table':'patent_inid_73','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},{'doc_field':'74','field_id':'74','inid':True,'field_type':'string','column_name':'inid_74','table':'patent_inid_74','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':'[;,](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},{'doc_field':'125','field_id':'125','inid':False,'field_type':'string','column_name':'f_125','table':'patent_f_125','ins_order':2,'ref_table':'patent','ref_field':'inid_11_id','fk':'patent_id','split_pattern':';','as_id':''},{'doc_field':'status','field_id':'127','inid':False,'field_type':'string','column_name':'f_127','table':'patent','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
       </c>
     </row>
   </sheetData>
@@ -2049,10 +2064,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2063,11 +2078,12 @@
     <col min="8" max="8" width="10.85546875" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" customWidth="1"/>
     <col min="11" max="11" width="37.42578125" customWidth="1"/>
-    <col min="12" max="12" width="29.42578125" customWidth="1"/>
-    <col min="13" max="13" width="35.7109375" customWidth="1"/>
+    <col min="12" max="12" width="6.85546875" customWidth="1"/>
+    <col min="13" max="13" width="29.42578125" customWidth="1"/>
+    <col min="14" max="14" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -2096,15 +2112,18 @@
         <v>35</v>
       </c>
       <c r="J1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s">
         <v>38</v>
       </c>
-      <c r="K1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>11</v>
@@ -2120,20 +2139,23 @@
         <v>f_11</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G2">
         <f>IF(F2="soft",1,2)</f>
         <v>1</v>
       </c>
-      <c r="L2" t="str">
-        <f>"{'"&amp;$A$1&amp;"':'"&amp;A2&amp;"',"&amp;"'"&amp;$B$1&amp;"':'"&amp;B2&amp;"',"&amp;"'"&amp;$C$1&amp;"':"&amp;C2&amp;","&amp;"'"&amp;$D$1&amp;"':'"&amp;D2&amp;"',"&amp;"'"&amp;$E$1&amp;"':'"&amp;E2&amp;"',"&amp;"'"&amp;$F$1&amp;"':'"&amp;F2&amp;"',"&amp;"'"&amp;$G$1&amp;"':"&amp;G2&amp;",'"&amp;$H$1&amp;"':'"&amp;H2&amp;"','"&amp;$I$1&amp;"':'"&amp;I2&amp;"','"&amp;$J$1&amp;"':'"&amp;J2&amp;"','"&amp;$K$1&amp;"':'"&amp;K2&amp;"'},"</f>
-        <v>{'doc_field':'Номер регистрации (свидетельства)','field_id':'11','inid':False,'field_type':'string','column_name':'f_11','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="str">
+        <f>"{'"&amp;$A$1&amp;"':'"&amp;A2&amp;"',"&amp;"'"&amp;$B$1&amp;"':'"&amp;B2&amp;"',"&amp;"'"&amp;$C$1&amp;"':"&amp;C2&amp;","&amp;"'"&amp;$D$1&amp;"':'"&amp;D2&amp;"',"&amp;"'"&amp;$E$1&amp;"':'"&amp;E2&amp;"',"&amp;"'"&amp;$F$1&amp;"':'"&amp;F2&amp;"',"&amp;"'"&amp;$G$1&amp;"':"&amp;G2&amp;",'"&amp;$H$1&amp;"':'"&amp;H2&amp;"','"&amp;$I$1&amp;"':'"&amp;I2&amp;"','"&amp;$J$1&amp;"':'"&amp;J2&amp;"','"&amp;$K$1&amp;"':'"&amp;K2&amp;"','"&amp;$L$1&amp;"':'"&amp;L2&amp;"'},"</f>
+        <v>{'doc_field':'Номер регистрации (свидетельства)','field_id':'11','inid':False,'field_type':'string','column_name':'f_11','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':'1'},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3">
         <v>12</v>
@@ -2149,20 +2171,20 @@
         <v>f_12</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G22" si="1">IF(F3="soft",1,2)</f>
         <v>1</v>
       </c>
-      <c r="L3" t="str">
-        <f t="shared" ref="L3:L22" si="2">"{'"&amp;$A$1&amp;"':'"&amp;A3&amp;"',"&amp;"'"&amp;$B$1&amp;"':'"&amp;B3&amp;"',"&amp;"'"&amp;$C$1&amp;"':"&amp;C3&amp;","&amp;"'"&amp;$D$1&amp;"':'"&amp;D3&amp;"',"&amp;"'"&amp;$E$1&amp;"':'"&amp;E3&amp;"',"&amp;"'"&amp;$F$1&amp;"':'"&amp;F3&amp;"',"&amp;"'"&amp;$G$1&amp;"':"&amp;G3&amp;",'"&amp;$H$1&amp;"':'"&amp;H3&amp;"','"&amp;$I$1&amp;"':'"&amp;I3&amp;"','"&amp;$J$1&amp;"':'"&amp;J3&amp;"','"&amp;$K$1&amp;"':'"&amp;K3&amp;"'},"</f>
-        <v>{'doc_field':'Cловесное обозначение вида документа','field_id':'12','inid':False,'field_type':'string','column_name':'f_12','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M22" si="2">"{'"&amp;$A$1&amp;"':'"&amp;A3&amp;"',"&amp;"'"&amp;$B$1&amp;"':'"&amp;B3&amp;"',"&amp;"'"&amp;$C$1&amp;"':"&amp;C3&amp;","&amp;"'"&amp;$D$1&amp;"':'"&amp;D3&amp;"',"&amp;"'"&amp;$E$1&amp;"':'"&amp;E3&amp;"',"&amp;"'"&amp;$F$1&amp;"':'"&amp;F3&amp;"',"&amp;"'"&amp;$G$1&amp;"':"&amp;G3&amp;",'"&amp;$H$1&amp;"':'"&amp;H3&amp;"','"&amp;$I$1&amp;"':'"&amp;I3&amp;"','"&amp;$J$1&amp;"':'"&amp;J3&amp;"','"&amp;$K$1&amp;"':'"&amp;K3&amp;"','"&amp;$L$1&amp;"':'"&amp;L3&amp;"'},"</f>
+        <v>{'doc_field':'Cловесное обозначение вида документа','field_id':'12','inid':False,'field_type':'string','column_name':'f_12','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4">
         <v>19</v>
@@ -2178,20 +2200,20 @@
         <v>f_19</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L4" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'Идентификация органа, регистрирующего программу ЭВМ/базу данных','field_id':'19','inid':False,'field_type':'string','column_name':'f_19','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Идентификация органа, регистрирующего программу ЭВМ/базу данных','field_id':'19','inid':False,'field_type':'string','column_name':'f_19','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>21</v>
@@ -2207,20 +2229,20 @@
         <v>f_21</v>
       </c>
       <c r="F5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L5" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'Номер заявки','field_id':'21','inid':False,'field_type':'string','column_name':'f_21','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Номер заявки','field_id':'21','inid':False,'field_type':'string','column_name':'f_21','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>22</v>
@@ -2236,20 +2258,20 @@
         <v>f_22</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L6" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'Дата поступления заявки','field_id':'22','inid':False,'field_type':'date','column_name':'f_22','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Дата поступления заявки','field_id':'22','inid':False,'field_type':'date','column_name':'f_22','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7">
         <v>24</v>
@@ -2265,20 +2287,20 @@
         <v>f_24</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L7" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'Дата регистрации','field_id':'24','inid':False,'field_type':'date','column_name':'f_24','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Дата регистрации','field_id':'24','inid':False,'field_type':'date','column_name':'f_24','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8">
         <v>45</v>
@@ -2294,20 +2316,20 @@
         <v>f_45</v>
       </c>
       <c r="F8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L8" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'Дата публикации','field_id':'45','inid':False,'field_type':'date','column_name':'f_45','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Дата публикации','field_id':'45','inid':False,'field_type':'date','column_name':'f_45','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9">
         <v>54</v>
@@ -2323,20 +2345,20 @@
         <v>f_54</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L9" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'Название программы ЭВМ/базы данных','field_id':'54','inid':False,'field_type':'string','column_name':'f_54','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Название программы ЭВМ/базы данных','field_id':'54','inid':False,'field_type':'string','column_name':'f_54','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10">
         <v>72</v>
@@ -2352,32 +2374,32 @@
         <v>f_72</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I10" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="J10" t="s">
+        <v>68</v>
+      </c>
+      <c r="K10" t="s">
         <v>69</v>
       </c>
-      <c r="K10" t="s">
-        <v>70</v>
-      </c>
-      <c r="L10" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'Автор','field_id':'72','inid':False,'field_type':'string','column_name':'f_72','table':'soft_f_72','ins_order':2,'ref_table':'soft','ref_field':'id','fk':'soft_id','split_pattern':'[;](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Автор','field_id':'72','inid':False,'field_type':'string','column_name':'f_72','table':'soft_f_72','ins_order':2,'ref_table':'soft','ref_field':'f_11_id','fk':'soft_id','split_pattern':'[;](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11">
         <v>73</v>
@@ -2393,32 +2415,32 @@
         <v>f_73</v>
       </c>
       <c r="F11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" t="s">
         <v>68</v>
       </c>
-      <c r="G11">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H11" t="s">
-        <v>66</v>
-      </c>
-      <c r="I11" t="s">
-        <v>37</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>69</v>
       </c>
-      <c r="K11" t="s">
-        <v>70</v>
-      </c>
-      <c r="L11" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'Правообладатель','field_id':'73','inid':False,'field_type':'string','column_name':'f_73','table':'soft_f_73','ins_order':2,'ref_table':'soft','ref_field':'id','fk':'soft_id','split_pattern':'[;](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))'},</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Правообладатель','field_id':'73','inid':False,'field_type':'string','column_name':'f_73','table':'soft_f_73','ins_order':2,'ref_table':'soft','ref_field':'f_11_id','fk':'soft_id','split_pattern':'[;](?!\\s*(?:ЛТД|ЭлЭлСи|ИНК|ЛЛК))','as_id':''},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12">
         <v>98</v>
@@ -2434,20 +2456,20 @@
         <v>f_98</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L12" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'Контактные реквизиты','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Контактные реквизиты','field_id':'98','inid':False,'field_type':'string','column_name':'f_98','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13">
         <v>111</v>
@@ -2463,20 +2485,20 @@
         <v>f_111</v>
       </c>
       <c r="F13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L13" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'Программа для ЭВМ/база данных создана по государственному контракту','field_id':'111','inid':False,'field_type':'string','column_name':'f_111','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Программа для ЭВМ/база данных создана по государственному контракту','field_id':'111','inid':False,'field_type':'string','column_name':'f_111','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14">
         <v>112</v>
@@ -2492,20 +2514,20 @@
         <v>f_112</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L14" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'Вид и версия операционной системы','field_id':'112','inid':False,'field_type':'string','column_name':'f_112','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Вид и версия операционной системы','field_id':'112','inid':False,'field_type':'string','column_name':'f_112','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15">
         <v>113</v>
@@ -2521,20 +2543,20 @@
         <v>f_113</v>
       </c>
       <c r="F15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L15" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'Язык программирования','field_id':'113','inid':False,'field_type':'string','column_name':'f_113','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Язык программирования','field_id':'113','inid':False,'field_type':'string','column_name':'f_113','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16">
         <v>114</v>
@@ -2550,20 +2572,20 @@
         <v>f_114</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L16" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'Вид и версия системы управления базой данных','field_id':'114','inid':False,'field_type':'string','column_name':'f_114','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Вид и версия системы управления базой данных','field_id':'114','inid':False,'field_type':'string','column_name':'f_114','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17">
         <v>115</v>
@@ -2579,20 +2601,20 @@
         <v>f_115</v>
       </c>
       <c r="F17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G17">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L17" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'Тип реализующей ЭВМ','field_id':'115','inid':False,'field_type':'string','column_name':'f_115','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Тип реализующей ЭВМ','field_id':'115','inid':False,'field_type':'string','column_name':'f_115','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18">
         <v>116</v>
@@ -2608,20 +2630,20 @@
         <v>f_116</v>
       </c>
       <c r="F18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L18" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'Объем программы для ЭВМ/базы данных','field_id':'116','inid':False,'field_type':'string','column_name':'f_116','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Объем программы для ЭВМ/базы данных','field_id':'116','inid':False,'field_type':'string','column_name':'f_116','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19">
         <v>121</v>
@@ -2637,20 +2659,20 @@
         <v>f_121</v>
       </c>
       <c r="F19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L19" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'Номер регистрации (свидетельства)_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Номер регистрации (свидетельства)_href','field_id':'121','inid':False,'field_type':'string','column_name':'f_121','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20">
         <v>124</v>
@@ -2666,20 +2688,20 @@
         <v>f_124</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L20" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'Дата публикации_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Дата публикации_href','field_id':'124','inid':False,'field_type':'string','column_name':'f_124','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21">
         <v>125</v>
@@ -2695,20 +2717,20 @@
         <v>f_125</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L21" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'Извещения об изменениях сведений','field_id':'125','inid':False,'field_type':'string','column_name':'f_125','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Извещения об изменениях сведений','field_id':'125','inid':False,'field_type':'string','column_name':'f_125','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22">
         <v>126</v>
@@ -2724,15 +2746,15 @@
         <v>f_126</v>
       </c>
       <c r="F22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L22" t="str">
-        <f t="shared" si="2"/>
-        <v>{'doc_field':'Извещения об изменениях сведений_href','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':''},</v>
+      <c r="M22" t="str">
+        <f t="shared" si="2"/>
+        <v>{'doc_field':'Извещения об изменениях сведений_href','field_id':'126','inid':False,'field_type':'string','column_name':'f_126','table':'soft','ins_order':1,'ref_table':'','ref_field':'','fk':'','split_pattern':'','as_id':''},</v>
       </c>
     </row>
   </sheetData>

</xml_diff>